<commit_message>
Modifico los archivos excel
</commit_message>
<xml_diff>
--- a/Inventariado Fisico.xlsx
+++ b/Inventariado Fisico.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lover\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pepit\Desktop\ProyectoFinal_Programacion3\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03FDDEB4-BD03-47C9-A98A-295864D73634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19550" windowHeight="8750"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="488">
   <si>
     <t>Grupo</t>
   </si>
@@ -1488,7 +1489,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1847,22 +1848,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H232"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C233" sqref="C233"/>
+      <selection activeCell="A231" sqref="A231:A232"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1888,7 +1889,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1906,8 +1907,10 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1922,8 +1925,10 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1938,7 +1943,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -1956,8 +1961,10 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
@@ -1972,8 +1979,10 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
@@ -1988,8 +1997,10 @@
       </c>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
@@ -2006,7 +2017,7 @@
       </c>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
@@ -2026,7 +2037,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -2044,8 +2055,10 @@
       </c>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="B11" s="2" t="s">
         <v>25</v>
       </c>
@@ -2062,8 +2075,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="B12" s="2" t="s">
         <v>27</v>
       </c>
@@ -2078,8 +2093,10 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="2"/>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="B13" s="2" t="s">
         <v>29</v>
       </c>
@@ -2096,8 +2113,10 @@
       </c>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="2"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="B14" s="2" t="s">
         <v>31</v>
       </c>
@@ -2112,8 +2131,10 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="2"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="B15" s="2" t="s">
         <v>33</v>
       </c>
@@ -2128,8 +2149,10 @@
       </c>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="2"/>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="B16" s="2" t="s">
         <v>35</v>
       </c>
@@ -2144,8 +2167,10 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="2"/>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="B17" s="2" t="s">
         <v>37</v>
       </c>
@@ -2160,8 +2185,10 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="2"/>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="B18" s="2" t="s">
         <v>39</v>
       </c>
@@ -2178,8 +2205,10 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="2"/>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="B19" s="2" t="s">
         <v>41</v>
       </c>
@@ -2194,8 +2223,10 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="2"/>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="B20" s="2" t="s">
         <v>43</v>
       </c>
@@ -2210,7 +2241,7 @@
       </c>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>45</v>
       </c>
@@ -2230,7 +2261,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>48</v>
       </c>
@@ -2250,8 +2281,10 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="2"/>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="B23" s="2" t="s">
         <v>51</v>
       </c>
@@ -2268,8 +2301,10 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="2"/>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="B24" s="2" t="s">
         <v>53</v>
       </c>
@@ -2286,8 +2321,10 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="2"/>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="B25" s="2" t="s">
         <v>55</v>
       </c>
@@ -2304,8 +2341,10 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="2"/>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="B26" s="2" t="s">
         <v>57</v>
       </c>
@@ -2320,8 +2359,10 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="2"/>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="B27" s="2" t="s">
         <v>59</v>
       </c>
@@ -2336,8 +2377,10 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="2"/>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="B28" s="2" t="s">
         <v>61</v>
       </c>
@@ -2352,8 +2395,10 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="2"/>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="B29" s="2" t="s">
         <v>63</v>
       </c>
@@ -2370,8 +2415,10 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="2"/>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="B30" s="2" t="s">
         <v>65</v>
       </c>
@@ -2388,8 +2435,10 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" s="2"/>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="B31" s="2" t="s">
         <v>67</v>
       </c>
@@ -2406,8 +2455,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" s="2"/>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="B32" s="2" t="s">
         <v>69</v>
       </c>
@@ -2424,8 +2475,10 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="2"/>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="B33" s="2" t="s">
         <v>71</v>
       </c>
@@ -2440,7 +2493,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>73</v>
       </c>
@@ -2458,8 +2511,10 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" s="2"/>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B35" s="2" t="s">
         <v>76</v>
       </c>
@@ -2474,8 +2529,10 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36" s="2"/>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B36" s="2" t="s">
         <v>78</v>
       </c>
@@ -2492,8 +2549,10 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A37" s="2"/>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B37" s="2" t="s">
         <v>80</v>
       </c>
@@ -2508,8 +2567,10 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A38" s="2"/>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B38" s="2" t="s">
         <v>82</v>
       </c>
@@ -2528,8 +2589,10 @@
       </c>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A39" s="2"/>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B39" s="2" t="s">
         <v>84</v>
       </c>
@@ -2548,8 +2611,10 @@
       </c>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A40" s="2"/>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B40" s="2" t="s">
         <v>86</v>
       </c>
@@ -2568,8 +2633,10 @@
       </c>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A41" s="2"/>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B41" s="2" t="s">
         <v>88</v>
       </c>
@@ -2586,8 +2653,10 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A42" s="2"/>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B42" s="2" t="s">
         <v>90</v>
       </c>
@@ -2604,8 +2673,10 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A43" s="2"/>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B43" s="2" t="s">
         <v>92</v>
       </c>
@@ -2620,8 +2691,10 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A44" s="2"/>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B44" s="2" t="s">
         <v>94</v>
       </c>
@@ -2636,8 +2709,10 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A45" s="2"/>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B45" s="2" t="s">
         <v>96</v>
       </c>
@@ -2654,8 +2729,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A46" s="2"/>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B46" s="2" t="s">
         <v>98</v>
       </c>
@@ -2674,8 +2751,10 @@
       </c>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A47" s="2"/>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B47" s="2" t="s">
         <v>100</v>
       </c>
@@ -2692,8 +2771,10 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A48" s="2"/>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B48" s="2" t="s">
         <v>102</v>
       </c>
@@ -2710,8 +2791,10 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A49" s="2"/>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B49" s="2" t="s">
         <v>104</v>
       </c>
@@ -2732,8 +2815,10 @@
       </c>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A50" s="2"/>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B50" s="2" t="s">
         <v>106</v>
       </c>
@@ -2748,8 +2833,10 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A51" s="2"/>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B51" s="2" t="s">
         <v>108</v>
       </c>
@@ -2766,8 +2853,10 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A52" s="2"/>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B52" s="2" t="s">
         <v>110</v>
       </c>
@@ -2786,8 +2875,10 @@
       </c>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A53" s="2"/>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B53" s="2" t="s">
         <v>112</v>
       </c>
@@ -2804,8 +2895,10 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A54" s="2"/>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B54" s="2" t="s">
         <v>114</v>
       </c>
@@ -2820,8 +2913,10 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A55" s="2"/>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B55" s="2" t="s">
         <v>116</v>
       </c>
@@ -2836,8 +2931,10 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A56" s="2"/>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B56" s="2" t="s">
         <v>118</v>
       </c>
@@ -2852,8 +2949,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A57" s="2"/>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B57" s="2" t="s">
         <v>120</v>
       </c>
@@ -2868,8 +2967,10 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A58" s="2"/>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B58" s="2" t="s">
         <v>122</v>
       </c>
@@ -2884,8 +2985,10 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A59" s="2"/>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B59" s="2" t="s">
         <v>124</v>
       </c>
@@ -2902,8 +3005,10 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A60" s="2"/>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B60" s="2" t="s">
         <v>126</v>
       </c>
@@ -2920,8 +3025,10 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A61" s="2"/>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B61" s="2" t="s">
         <v>128</v>
       </c>
@@ -2940,8 +3047,10 @@
       </c>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A62" s="2"/>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B62" s="2" t="s">
         <v>130</v>
       </c>
@@ -2956,8 +3065,10 @@
       </c>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A63" s="2"/>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B63" s="2" t="s">
         <v>132</v>
       </c>
@@ -2972,8 +3083,10 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A64" s="2"/>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B64" s="2" t="s">
         <v>134</v>
       </c>
@@ -2988,8 +3101,10 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A65" s="2"/>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B65" s="2" t="s">
         <v>136</v>
       </c>
@@ -3004,8 +3119,10 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A66" s="2"/>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B66" s="2" t="s">
         <v>138</v>
       </c>
@@ -3022,8 +3139,10 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A67" s="2"/>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B67" s="2" t="s">
         <v>140</v>
       </c>
@@ -3038,8 +3157,10 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A68" s="2"/>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B68" s="2" t="s">
         <v>142</v>
       </c>
@@ -3056,8 +3177,10 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A69" s="2"/>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B69" s="2" t="s">
         <v>144</v>
       </c>
@@ -3074,8 +3197,10 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A70" s="2"/>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B70" s="2" t="s">
         <v>146</v>
       </c>
@@ -3092,8 +3217,10 @@
       </c>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A71" s="2"/>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B71" s="2" t="s">
         <v>148</v>
       </c>
@@ -3108,8 +3235,10 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A72" s="2"/>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B72" s="2" t="s">
         <v>150</v>
       </c>
@@ -3126,8 +3255,10 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A73" s="2"/>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B73" s="2" t="s">
         <v>152</v>
       </c>
@@ -3144,8 +3275,10 @@
       </c>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A74" s="2"/>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B74" s="2" t="s">
         <v>154</v>
       </c>
@@ -3160,8 +3293,10 @@
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A75" s="2"/>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B75" s="2" t="s">
         <v>156</v>
       </c>
@@ -3178,8 +3313,10 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A76" s="2"/>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B76" s="2" t="s">
         <v>158</v>
       </c>
@@ -3196,8 +3333,10 @@
       </c>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A77" s="2"/>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B77" s="2" t="s">
         <v>160</v>
       </c>
@@ -3214,8 +3353,10 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A78" s="2"/>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B78" s="2" t="s">
         <v>162</v>
       </c>
@@ -3232,8 +3373,10 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A79" s="2"/>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B79" s="2" t="s">
         <v>164</v>
       </c>
@@ -3250,8 +3393,10 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A80" s="2"/>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B80" s="2" t="s">
         <v>166</v>
       </c>
@@ -3268,8 +3413,10 @@
       </c>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A81" s="2"/>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B81" s="2" t="s">
         <v>168</v>
       </c>
@@ -3290,8 +3437,10 @@
       </c>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A82" s="2"/>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B82" s="2" t="s">
         <v>170</v>
       </c>
@@ -3308,8 +3457,10 @@
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A83" s="2"/>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B83" s="2" t="s">
         <v>172</v>
       </c>
@@ -3328,8 +3479,10 @@
       </c>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A84" s="2"/>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B84" s="2" t="s">
         <v>174</v>
       </c>
@@ -3346,8 +3499,10 @@
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A85" s="2"/>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B85" s="2" t="s">
         <v>176</v>
       </c>
@@ -3368,8 +3523,10 @@
       </c>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A86" s="2"/>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B86" s="2" t="s">
         <v>178</v>
       </c>
@@ -3384,8 +3541,10 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A87" s="2"/>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B87" s="2" t="s">
         <v>180</v>
       </c>
@@ -3404,8 +3563,10 @@
       </c>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A88" s="2"/>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B88" s="2" t="s">
         <v>182</v>
       </c>
@@ -3422,8 +3583,10 @@
       </c>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A89" s="2"/>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B89" s="2" t="s">
         <v>184</v>
       </c>
@@ -3442,8 +3605,10 @@
       </c>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A90" s="2"/>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B90" s="2" t="s">
         <v>186</v>
       </c>
@@ -3462,8 +3627,10 @@
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A91" s="2"/>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B91" s="2" t="s">
         <v>188</v>
       </c>
@@ -3480,8 +3647,10 @@
       </c>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A92" s="2"/>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B92" s="2" t="s">
         <v>190</v>
       </c>
@@ -3498,8 +3667,10 @@
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A93" s="2"/>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B93" s="2" t="s">
         <v>192</v>
       </c>
@@ -3514,8 +3685,10 @@
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A94" s="2"/>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B94" s="2" t="s">
         <v>194</v>
       </c>
@@ -3532,7 +3705,7 @@
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>196</v>
       </c>
@@ -3552,8 +3725,10 @@
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A96" s="2"/>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>196</v>
+      </c>
       <c r="B96" s="2" t="s">
         <v>199</v>
       </c>
@@ -3570,8 +3745,10 @@
       </c>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A97" s="2"/>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>196</v>
+      </c>
       <c r="B97" s="2" t="s">
         <v>201</v>
       </c>
@@ -3588,7 +3765,7 @@
       </c>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>203</v>
       </c>
@@ -3606,8 +3783,10 @@
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A99" s="2"/>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>203</v>
+      </c>
       <c r="B99" s="2" t="s">
         <v>206</v>
       </c>
@@ -3622,8 +3801,10 @@
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A100" s="2"/>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
+        <v>203</v>
+      </c>
       <c r="B100" s="2" t="s">
         <v>208</v>
       </c>
@@ -3638,8 +3819,10 @@
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A101" s="2"/>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>203</v>
+      </c>
       <c r="B101" s="2" t="s">
         <v>210</v>
       </c>
@@ -3654,8 +3837,10 @@
       <c r="G101" s="2"/>
       <c r="H101" s="2"/>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A102" s="2"/>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
+        <v>203</v>
+      </c>
       <c r="B102" s="2" t="s">
         <v>212</v>
       </c>
@@ -3670,8 +3855,10 @@
       <c r="G102" s="2"/>
       <c r="H102" s="2"/>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A103" s="2"/>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>203</v>
+      </c>
       <c r="B103" s="2" t="s">
         <v>214</v>
       </c>
@@ -3688,8 +3875,10 @@
       </c>
       <c r="H103" s="2"/>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A104" s="2"/>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>203</v>
+      </c>
       <c r="B104" s="2" t="s">
         <v>216</v>
       </c>
@@ -3706,8 +3895,10 @@
       <c r="G104" s="2"/>
       <c r="H104" s="2"/>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A105" s="2"/>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
+        <v>203</v>
+      </c>
       <c r="B105" s="2" t="s">
         <v>218</v>
       </c>
@@ -3722,8 +3913,10 @@
       <c r="G105" s="2"/>
       <c r="H105" s="2"/>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A106" s="2"/>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
+        <v>203</v>
+      </c>
       <c r="B106" s="2" t="s">
         <v>220</v>
       </c>
@@ -3740,8 +3933,10 @@
       <c r="G106" s="2"/>
       <c r="H106" s="2"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A107" s="2"/>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
+        <v>203</v>
+      </c>
       <c r="B107" s="2" t="s">
         <v>222</v>
       </c>
@@ -3756,7 +3951,7 @@
       </c>
       <c r="H107" s="2"/>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>224</v>
       </c>
@@ -3774,8 +3969,10 @@
       <c r="G108" s="2"/>
       <c r="H108" s="2"/>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A109" s="2"/>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
+        <v>224</v>
+      </c>
       <c r="B109" s="2" t="s">
         <v>227</v>
       </c>
@@ -3792,8 +3989,10 @@
       <c r="G109" s="2"/>
       <c r="H109" s="2"/>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A110" s="2"/>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
+        <v>224</v>
+      </c>
       <c r="B110" s="2" t="s">
         <v>229</v>
       </c>
@@ -3808,8 +4007,10 @@
       <c r="G110" s="2"/>
       <c r="H110" s="2"/>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A111" s="2"/>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
+        <v>224</v>
+      </c>
       <c r="B111" s="2" t="s">
         <v>231</v>
       </c>
@@ -3826,8 +4027,10 @@
       <c r="G111" s="2"/>
       <c r="H111" s="2"/>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A112" s="2"/>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
+        <v>224</v>
+      </c>
       <c r="B112" s="2" t="s">
         <v>233</v>
       </c>
@@ -3842,8 +4045,10 @@
       <c r="G112" s="2"/>
       <c r="H112" s="2"/>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A113" s="2"/>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
+        <v>224</v>
+      </c>
       <c r="B113" s="2" t="s">
         <v>235</v>
       </c>
@@ -3860,8 +4065,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A114" s="2"/>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
+        <v>224</v>
+      </c>
       <c r="B114" s="2" t="s">
         <v>237</v>
       </c>
@@ -3876,8 +4083,10 @@
       <c r="G114" s="2"/>
       <c r="H114" s="2"/>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A115" s="2"/>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
+        <v>224</v>
+      </c>
       <c r="B115" s="2" t="s">
         <v>239</v>
       </c>
@@ -3894,8 +4103,10 @@
       <c r="G115" s="2"/>
       <c r="H115" s="2"/>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A116" s="2"/>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
+        <v>224</v>
+      </c>
       <c r="B116" s="2" t="s">
         <v>241</v>
       </c>
@@ -3910,8 +4121,10 @@
       <c r="G116" s="2"/>
       <c r="H116" s="2"/>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A117" s="2"/>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
+        <v>224</v>
+      </c>
       <c r="B117" s="2" t="s">
         <v>243</v>
       </c>
@@ -3928,8 +4141,10 @@
       <c r="G117" s="2"/>
       <c r="H117" s="2"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A118" s="2"/>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
+        <v>224</v>
+      </c>
       <c r="B118" s="2" t="s">
         <v>245</v>
       </c>
@@ -3944,8 +4159,10 @@
       <c r="G118" s="2"/>
       <c r="H118" s="2"/>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A119" s="2"/>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
+        <v>224</v>
+      </c>
       <c r="B119" s="2" t="s">
         <v>247</v>
       </c>
@@ -3960,8 +4177,10 @@
       <c r="G119" s="2"/>
       <c r="H119" s="2"/>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A120" s="2"/>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
+        <v>224</v>
+      </c>
       <c r="B120" s="2" t="s">
         <v>249</v>
       </c>
@@ -3976,8 +4195,10 @@
       <c r="G120" s="2"/>
       <c r="H120" s="2"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A121" s="2"/>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
+        <v>224</v>
+      </c>
       <c r="B121" s="2" t="s">
         <v>251</v>
       </c>
@@ -3992,8 +4213,10 @@
       <c r="G121" s="2"/>
       <c r="H121" s="2"/>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A122" s="2"/>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
+        <v>224</v>
+      </c>
       <c r="B122" s="2" t="s">
         <v>253</v>
       </c>
@@ -4008,8 +4231,10 @@
       <c r="G122" s="2"/>
       <c r="H122" s="2"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A123" s="2"/>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
+        <v>224</v>
+      </c>
       <c r="B123" s="2" t="s">
         <v>255</v>
       </c>
@@ -4024,8 +4249,10 @@
       <c r="G123" s="2"/>
       <c r="H123" s="2"/>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A124" s="2"/>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
+        <v>224</v>
+      </c>
       <c r="B124" s="2" t="s">
         <v>257</v>
       </c>
@@ -4040,8 +4267,10 @@
       <c r="G124" s="2"/>
       <c r="H124" s="2"/>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A125" s="2"/>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
+        <v>224</v>
+      </c>
       <c r="B125" s="2" t="s">
         <v>259</v>
       </c>
@@ -4056,7 +4285,7 @@
       <c r="G125" s="2"/>
       <c r="H125" s="2"/>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>261</v>
       </c>
@@ -4074,8 +4303,10 @@
       <c r="G126" s="2"/>
       <c r="H126" s="2"/>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A127" s="2"/>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A127" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="B127" s="2" t="s">
         <v>264</v>
       </c>
@@ -4092,8 +4323,10 @@
       <c r="G127" s="2"/>
       <c r="H127" s="2"/>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A128" s="2"/>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A128" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="B128" s="2" t="s">
         <v>266</v>
       </c>
@@ -4112,8 +4345,10 @@
       <c r="G128" s="2"/>
       <c r="H128" s="2"/>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A129" s="2"/>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A129" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="B129" s="2" t="s">
         <v>268</v>
       </c>
@@ -4130,8 +4365,10 @@
       <c r="G129" s="2"/>
       <c r="H129" s="2"/>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A130" s="2"/>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="B130" s="2" t="s">
         <v>270</v>
       </c>
@@ -4148,8 +4385,10 @@
       <c r="G130" s="2"/>
       <c r="H130" s="2"/>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A131" s="2"/>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A131" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="B131" s="2" t="s">
         <v>272</v>
       </c>
@@ -4164,8 +4403,10 @@
       </c>
       <c r="H131" s="2"/>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A132" s="2"/>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A132" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="B132" s="2" t="s">
         <v>274</v>
       </c>
@@ -4182,8 +4423,10 @@
       <c r="G132" s="2"/>
       <c r="H132" s="2"/>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A133" s="2"/>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A133" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="B133" s="2" t="s">
         <v>276</v>
       </c>
@@ -4198,8 +4441,10 @@
       </c>
       <c r="H133" s="2"/>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A134" s="2"/>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A134" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="B134" s="2" t="s">
         <v>278</v>
       </c>
@@ -4216,8 +4461,10 @@
       <c r="G134" s="2"/>
       <c r="H134" s="2"/>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A135" s="2"/>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="B135" s="2" t="s">
         <v>280</v>
       </c>
@@ -4234,8 +4481,10 @@
       <c r="G135" s="2"/>
       <c r="H135" s="2"/>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A136" s="2"/>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="B136" s="2" t="s">
         <v>282</v>
       </c>
@@ -4252,8 +4501,10 @@
       <c r="G136" s="2"/>
       <c r="H136" s="2"/>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A137" s="2"/>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A137" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="B137" s="2" t="s">
         <v>284</v>
       </c>
@@ -4270,8 +4521,10 @@
       <c r="G137" s="2"/>
       <c r="H137" s="2"/>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A138" s="2"/>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A138" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="B138" s="2" t="s">
         <v>286</v>
       </c>
@@ -4286,8 +4539,10 @@
       <c r="G138" s="2"/>
       <c r="H138" s="2"/>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A139" s="2"/>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="B139" s="2" t="s">
         <v>288</v>
       </c>
@@ -4304,8 +4559,10 @@
       <c r="G139" s="2"/>
       <c r="H139" s="2"/>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A140" s="2"/>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="B140" s="2" t="s">
         <v>290</v>
       </c>
@@ -4320,8 +4577,10 @@
       <c r="G140" s="2"/>
       <c r="H140" s="2"/>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A141" s="2"/>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="B141" s="2" t="s">
         <v>292</v>
       </c>
@@ -4338,8 +4597,10 @@
       <c r="G141" s="2"/>
       <c r="H141" s="2"/>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A142" s="2"/>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A142" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="B142" s="2" t="s">
         <v>294</v>
       </c>
@@ -4356,8 +4617,10 @@
       <c r="G142" s="2"/>
       <c r="H142" s="2"/>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A143" s="2"/>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="B143" s="2" t="s">
         <v>296</v>
       </c>
@@ -4374,8 +4637,10 @@
       <c r="G143" s="2"/>
       <c r="H143" s="2"/>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A144" s="2"/>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="B144" s="2" t="s">
         <v>298</v>
       </c>
@@ -4390,8 +4655,10 @@
       <c r="G144" s="2"/>
       <c r="H144" s="2"/>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A145" s="2"/>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="B145" s="2" t="s">
         <v>300</v>
       </c>
@@ -4406,8 +4673,10 @@
       <c r="G145" s="2"/>
       <c r="H145" s="2"/>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A146" s="2"/>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A146" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="B146" s="2" t="s">
         <v>302</v>
       </c>
@@ -4424,8 +4693,10 @@
       <c r="G146" s="2"/>
       <c r="H146" s="2"/>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A147" s="2"/>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A147" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="B147" s="2" t="s">
         <v>304</v>
       </c>
@@ -4442,8 +4713,10 @@
       <c r="G147" s="2"/>
       <c r="H147" s="2"/>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A148" s="2"/>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A148" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="B148" s="2" t="s">
         <v>306</v>
       </c>
@@ -4458,8 +4731,10 @@
       <c r="G148" s="2"/>
       <c r="H148" s="2"/>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A149" s="2"/>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A149" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="B149" s="2" t="s">
         <v>308</v>
       </c>
@@ -4476,8 +4751,10 @@
       <c r="G149" s="2"/>
       <c r="H149" s="2"/>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A150" s="2"/>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A150" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="B150" s="2" t="s">
         <v>310</v>
       </c>
@@ -4494,8 +4771,10 @@
       <c r="G150" s="2"/>
       <c r="H150" s="2"/>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A151" s="2"/>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A151" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="B151" s="2" t="s">
         <v>312</v>
       </c>
@@ -4512,8 +4791,10 @@
       <c r="G151" s="2"/>
       <c r="H151" s="2"/>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A152" s="2"/>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A152" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="B152" s="2" t="s">
         <v>314</v>
       </c>
@@ -4530,8 +4811,10 @@
       <c r="G152" s="2"/>
       <c r="H152" s="2"/>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A153" s="2"/>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A153" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="B153" s="2" t="s">
         <v>316</v>
       </c>
@@ -4550,8 +4833,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A154" s="2"/>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A154" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="B154" s="2" t="s">
         <v>318</v>
       </c>
@@ -4568,8 +4853,10 @@
       <c r="G154" s="2"/>
       <c r="H154" s="2"/>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A155" s="2"/>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A155" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="B155" s="2" t="s">
         <v>320</v>
       </c>
@@ -4586,8 +4873,10 @@
       <c r="G155" s="2"/>
       <c r="H155" s="2"/>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A156" s="2"/>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A156" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="B156" s="2" t="s">
         <v>322</v>
       </c>
@@ -4604,8 +4893,10 @@
       <c r="G156" s="2"/>
       <c r="H156" s="2"/>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A157" s="2"/>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A157" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="B157" s="2" t="s">
         <v>324</v>
       </c>
@@ -4622,8 +4913,10 @@
       <c r="G157" s="2"/>
       <c r="H157" s="2"/>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A158" s="2"/>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A158" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="B158" s="2" t="s">
         <v>326</v>
       </c>
@@ -4640,8 +4933,10 @@
       <c r="G158" s="2"/>
       <c r="H158" s="2"/>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A159" s="2"/>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A159" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="B159" s="2" t="s">
         <v>328</v>
       </c>
@@ -4658,8 +4953,10 @@
       <c r="G159" s="2"/>
       <c r="H159" s="2"/>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A160" s="2"/>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A160" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="B160" s="2" t="s">
         <v>330</v>
       </c>
@@ -4676,7 +4973,7 @@
       <c r="G160" s="2"/>
       <c r="H160" s="2"/>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>332</v>
       </c>
@@ -4696,8 +4993,10 @@
       </c>
       <c r="H161" s="2"/>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A162" s="2"/>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A162" s="2" t="s">
+        <v>332</v>
+      </c>
       <c r="B162" s="2" t="s">
         <v>335</v>
       </c>
@@ -4714,8 +5013,10 @@
       <c r="G162" s="2"/>
       <c r="H162" s="2"/>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A163" s="2"/>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A163" s="2" t="s">
+        <v>332</v>
+      </c>
       <c r="B163" s="2" t="s">
         <v>337</v>
       </c>
@@ -4730,8 +5031,10 @@
       <c r="G163" s="2"/>
       <c r="H163" s="2"/>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A164" s="2"/>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A164" s="2" t="s">
+        <v>332</v>
+      </c>
       <c r="B164" s="2" t="s">
         <v>339</v>
       </c>
@@ -4748,8 +5051,10 @@
       <c r="G164" s="2"/>
       <c r="H164" s="2"/>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A165" s="2"/>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A165" s="2" t="s">
+        <v>332</v>
+      </c>
       <c r="B165" s="2" t="s">
         <v>341</v>
       </c>
@@ -4764,8 +5069,10 @@
       <c r="G165" s="2"/>
       <c r="H165" s="2"/>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A166" s="2"/>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A166" s="2" t="s">
+        <v>332</v>
+      </c>
       <c r="B166" s="2" t="s">
         <v>343</v>
       </c>
@@ -4780,8 +5087,10 @@
       <c r="G166" s="2"/>
       <c r="H166" s="2"/>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A167" s="2"/>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A167" s="2" t="s">
+        <v>332</v>
+      </c>
       <c r="B167" s="2" t="s">
         <v>345</v>
       </c>
@@ -4796,8 +5105,10 @@
       <c r="G167" s="2"/>
       <c r="H167" s="2"/>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A168" s="2"/>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A168" s="2" t="s">
+        <v>332</v>
+      </c>
       <c r="B168" s="2" t="s">
         <v>347</v>
       </c>
@@ -4814,8 +5125,10 @@
       <c r="G168" s="2"/>
       <c r="H168" s="2"/>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A169" s="2"/>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A169" s="2" t="s">
+        <v>332</v>
+      </c>
       <c r="B169" s="2" t="s">
         <v>349</v>
       </c>
@@ -4830,8 +5143,10 @@
       <c r="G169" s="2"/>
       <c r="H169" s="2"/>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A170" s="2"/>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A170" s="2" t="s">
+        <v>332</v>
+      </c>
       <c r="B170" s="2" t="s">
         <v>351</v>
       </c>
@@ -4846,7 +5161,7 @@
       <c r="G170" s="2"/>
       <c r="H170" s="2"/>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>353</v>
       </c>
@@ -4868,8 +5183,10 @@
       </c>
       <c r="H171" s="2"/>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A172" s="2"/>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A172" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B172" s="2" t="s">
         <v>356</v>
       </c>
@@ -4886,8 +5203,10 @@
       </c>
       <c r="H172" s="2"/>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A173" s="2"/>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A173" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B173" s="2" t="s">
         <v>358</v>
       </c>
@@ -4906,8 +5225,10 @@
       </c>
       <c r="H173" s="2"/>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A174" s="2"/>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A174" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B174" s="2" t="s">
         <v>360</v>
       </c>
@@ -4928,8 +5249,10 @@
       </c>
       <c r="H174" s="2"/>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A175" s="2"/>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A175" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B175" s="2" t="s">
         <v>362</v>
       </c>
@@ -4948,8 +5271,10 @@
       </c>
       <c r="H175" s="2"/>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A176" s="2"/>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A176" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B176" s="2" t="s">
         <v>364</v>
       </c>
@@ -4968,8 +5293,10 @@
       </c>
       <c r="H176" s="2"/>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A177" s="2"/>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A177" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B177" s="2" t="s">
         <v>366</v>
       </c>
@@ -4984,8 +5311,10 @@
       <c r="G177" s="2"/>
       <c r="H177" s="2"/>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A178" s="2"/>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A178" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B178" s="2" t="s">
         <v>368</v>
       </c>
@@ -5000,8 +5329,10 @@
       </c>
       <c r="H178" s="2"/>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A179" s="2"/>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A179" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B179" s="2" t="s">
         <v>370</v>
       </c>
@@ -5016,8 +5347,10 @@
       </c>
       <c r="H179" s="2"/>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A180" s="2"/>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A180" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B180" s="2" t="s">
         <v>372</v>
       </c>
@@ -5032,8 +5365,10 @@
       <c r="G180" s="2"/>
       <c r="H180" s="2"/>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A181" s="2"/>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A181" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B181" s="2" t="s">
         <v>374</v>
       </c>
@@ -5048,8 +5383,10 @@
       <c r="G181" s="2"/>
       <c r="H181" s="2"/>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A182" s="2"/>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A182" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B182" s="2" t="s">
         <v>376</v>
       </c>
@@ -5066,8 +5403,10 @@
       </c>
       <c r="H182" s="2"/>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A183" s="2"/>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A183" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B183" s="2" t="s">
         <v>378</v>
       </c>
@@ -5082,8 +5421,10 @@
       <c r="G183" s="2"/>
       <c r="H183" s="2"/>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A184" s="2"/>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A184" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B184" s="2" t="s">
         <v>380</v>
       </c>
@@ -5098,8 +5439,10 @@
       </c>
       <c r="H184" s="2"/>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A185" s="2"/>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A185" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B185" s="2" t="s">
         <v>382</v>
       </c>
@@ -5114,8 +5457,10 @@
       <c r="G185" s="2"/>
       <c r="H185" s="2"/>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A186" s="2"/>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A186" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B186" s="2" t="s">
         <v>384</v>
       </c>
@@ -5130,8 +5475,10 @@
       <c r="G186" s="2"/>
       <c r="H186" s="2"/>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A187" s="2"/>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A187" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B187" s="2" t="s">
         <v>386</v>
       </c>
@@ -5146,8 +5493,10 @@
       <c r="G187" s="2"/>
       <c r="H187" s="2"/>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A188" s="2"/>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A188" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B188" s="2" t="s">
         <v>388</v>
       </c>
@@ -5162,8 +5511,10 @@
       <c r="G188" s="2"/>
       <c r="H188" s="2"/>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A189" s="2"/>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A189" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B189" s="2" t="s">
         <v>390</v>
       </c>
@@ -5180,8 +5531,10 @@
       <c r="G189" s="2"/>
       <c r="H189" s="2"/>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A190" s="2"/>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A190" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B190" s="2" t="s">
         <v>392</v>
       </c>
@@ -5198,8 +5551,10 @@
       <c r="G190" s="2"/>
       <c r="H190" s="2"/>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A191" s="2"/>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A191" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B191" s="2" t="s">
         <v>394</v>
       </c>
@@ -5216,8 +5571,10 @@
       <c r="G191" s="2"/>
       <c r="H191" s="2"/>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A192" s="2"/>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A192" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B192" s="2" t="s">
         <v>396</v>
       </c>
@@ -5232,8 +5589,10 @@
       <c r="G192" s="2"/>
       <c r="H192" s="2"/>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A193" s="2"/>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A193" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B193" s="2" t="s">
         <v>398</v>
       </c>
@@ -5248,8 +5607,10 @@
       <c r="G193" s="2"/>
       <c r="H193" s="2"/>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A194" s="2"/>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A194" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B194" s="2" t="s">
         <v>400</v>
       </c>
@@ -5266,8 +5627,10 @@
       </c>
       <c r="H194" s="2"/>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A195" s="2"/>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A195" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B195" s="2" t="s">
         <v>402</v>
       </c>
@@ -5282,8 +5645,10 @@
       <c r="G195" s="2"/>
       <c r="H195" s="2"/>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A196" s="2"/>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A196" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B196" s="2" t="s">
         <v>404</v>
       </c>
@@ -5298,8 +5663,10 @@
       <c r="G196" s="2"/>
       <c r="H196" s="2"/>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A197" s="2"/>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A197" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B197" s="2" t="s">
         <v>406</v>
       </c>
@@ -5314,8 +5681,10 @@
       <c r="G197" s="2"/>
       <c r="H197" s="2"/>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A198" s="2"/>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A198" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B198" s="2" t="s">
         <v>408</v>
       </c>
@@ -5330,8 +5699,10 @@
       <c r="G198" s="2"/>
       <c r="H198" s="2"/>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A199" s="2"/>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A199" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B199" s="2" t="s">
         <v>410</v>
       </c>
@@ -5346,8 +5717,10 @@
       <c r="G199" s="2"/>
       <c r="H199" s="2"/>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A200" s="2"/>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A200" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B200" s="2" t="s">
         <v>412</v>
       </c>
@@ -5364,8 +5737,10 @@
       <c r="G200" s="2"/>
       <c r="H200" s="2"/>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A201" s="2"/>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A201" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B201" s="2" t="s">
         <v>414</v>
       </c>
@@ -5384,8 +5759,10 @@
       </c>
       <c r="H201" s="2"/>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A202" s="2"/>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A202" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B202" s="2" t="s">
         <v>416</v>
       </c>
@@ -5404,8 +5781,10 @@
       </c>
       <c r="H202" s="2"/>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A203" s="2"/>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A203" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B203" s="2" t="s">
         <v>418</v>
       </c>
@@ -5420,8 +5799,10 @@
       <c r="G203" s="2"/>
       <c r="H203" s="2"/>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A204" s="2"/>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A204" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B204" s="2" t="s">
         <v>420</v>
       </c>
@@ -5436,8 +5817,10 @@
       <c r="G204" s="2"/>
       <c r="H204" s="2"/>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A205" s="2"/>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A205" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B205" s="2" t="s">
         <v>422</v>
       </c>
@@ -5452,8 +5835,10 @@
       <c r="G205" s="2"/>
       <c r="H205" s="2"/>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A206" s="2"/>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A206" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B206" s="2" t="s">
         <v>424</v>
       </c>
@@ -5468,8 +5853,10 @@
       </c>
       <c r="H206" s="2"/>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A207" s="2"/>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A207" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B207" s="2" t="s">
         <v>426</v>
       </c>
@@ -5484,8 +5871,10 @@
       <c r="G207" s="2"/>
       <c r="H207" s="2"/>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A208" s="2"/>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A208" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B208" s="2" t="s">
         <v>428</v>
       </c>
@@ -5500,8 +5889,10 @@
       </c>
       <c r="H208" s="2"/>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A209" s="2"/>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A209" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B209" s="2" t="s">
         <v>430</v>
       </c>
@@ -5516,8 +5907,10 @@
       <c r="G209" s="2"/>
       <c r="H209" s="2"/>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A210" s="2"/>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A210" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B210" s="2" t="s">
         <v>432</v>
       </c>
@@ -5532,8 +5925,10 @@
       <c r="G210" s="2"/>
       <c r="H210" s="2"/>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A211" s="2"/>
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A211" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B211" s="2" t="s">
         <v>434</v>
       </c>
@@ -5552,8 +5947,10 @@
       </c>
       <c r="H211" s="2"/>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A212" s="2"/>
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A212" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B212" s="2" t="s">
         <v>436</v>
       </c>
@@ -5568,8 +5965,10 @@
       <c r="G212" s="2"/>
       <c r="H212" s="2"/>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A213" s="2"/>
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A213" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B213" s="2" t="s">
         <v>438</v>
       </c>
@@ -5586,8 +5985,10 @@
       <c r="G213" s="2"/>
       <c r="H213" s="2"/>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A214" s="2"/>
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A214" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B214" s="2" t="s">
         <v>440</v>
       </c>
@@ -5604,8 +6005,10 @@
       <c r="G214" s="2"/>
       <c r="H214" s="2"/>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A215" s="2"/>
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A215" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B215" s="2" t="s">
         <v>442</v>
       </c>
@@ -5622,8 +6025,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A216" s="2"/>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A216" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B216" s="2" t="s">
         <v>444</v>
       </c>
@@ -5640,8 +6045,10 @@
       <c r="G216" s="2"/>
       <c r="H216" s="2"/>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A217" s="2"/>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A217" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B217" s="2" t="s">
         <v>446</v>
       </c>
@@ -5656,8 +6063,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A218" s="2"/>
+    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A218" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B218" s="2" t="s">
         <v>448</v>
       </c>
@@ -5672,8 +6081,10 @@
       <c r="G218" s="2"/>
       <c r="H218" s="2"/>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A219" s="2"/>
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A219" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B219" s="2" t="s">
         <v>450</v>
       </c>
@@ -5690,8 +6101,10 @@
       <c r="G219" s="2"/>
       <c r="H219" s="2"/>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A220" s="2"/>
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A220" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B220" s="2" t="s">
         <v>452</v>
       </c>
@@ -5706,8 +6119,10 @@
       <c r="G220" s="2"/>
       <c r="H220" s="2"/>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A221" s="2"/>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A221" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B221" s="2" t="s">
         <v>454</v>
       </c>
@@ -5726,8 +6141,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A222" s="2"/>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A222" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B222" s="2" t="s">
         <v>456</v>
       </c>
@@ -5742,8 +6159,10 @@
       <c r="G222" s="2"/>
       <c r="H222" s="2"/>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A223" s="2"/>
+    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A223" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="B223" s="2" t="s">
         <v>458</v>
       </c>
@@ -5758,7 +6177,7 @@
       <c r="G223" s="2"/>
       <c r="H223" s="2"/>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
         <v>460</v>
       </c>
@@ -5776,8 +6195,10 @@
       <c r="G224" s="2"/>
       <c r="H224" s="2"/>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A225" s="2"/>
+    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A225" s="2" t="s">
+        <v>460</v>
+      </c>
       <c r="B225" s="2" t="s">
         <v>463</v>
       </c>
@@ -5792,8 +6213,10 @@
       <c r="G225" s="2"/>
       <c r="H225" s="2"/>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A226" s="2"/>
+    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A226" s="2" t="s">
+        <v>460</v>
+      </c>
       <c r="B226" s="2" t="s">
         <v>465</v>
       </c>
@@ -5808,7 +6231,7 @@
       <c r="G226" s="2"/>
       <c r="H226" s="2"/>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
         <v>467</v>
       </c>
@@ -5826,7 +6249,7 @@
       <c r="G227" s="2"/>
       <c r="H227" s="2"/>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
         <v>470</v>
       </c>
@@ -5844,8 +6267,10 @@
       <c r="G228" s="2"/>
       <c r="H228" s="2"/>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A229" s="2"/>
+    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A229" s="2" t="s">
+        <v>470</v>
+      </c>
       <c r="B229" s="2" t="s">
         <v>473</v>
       </c>
@@ -5860,7 +6285,7 @@
       <c r="G229" s="2"/>
       <c r="H229" s="2"/>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
         <v>475</v>
       </c>
@@ -5878,7 +6303,7 @@
       <c r="G230" s="2"/>
       <c r="H230" s="2"/>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
         <v>478</v>
       </c>
@@ -5896,8 +6321,10 @@
       <c r="G231" s="2"/>
       <c r="H231" s="2"/>
     </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A232" s="2"/>
+    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A232" s="2" t="s">
+        <v>478</v>
+      </c>
       <c r="B232" s="2" t="s">
         <v>481</v>
       </c>

</xml_diff>

<commit_message>
Co-authored-by: Rous444 <Rous444@users.noreply.github.com> Co-authored-by: frantmateos <frantmateos@users.noreply.github.com> Co-authored-by: pepitomorzila <pepitomorzila@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Inventariado Fisico.xlsx
+++ b/Inventariado Fisico.xlsx
@@ -1883,7 +1883,7 @@
     <col min="8" max="8" style="6" width="9.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -1927,7 +1927,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -1945,7 +1945,7 @@
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -1963,7 +1963,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -1981,7 +1981,7 @@
       </c>
       <c r="H5" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
@@ -1999,7 +1999,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -2017,7 +2017,7 @@
       </c>
       <c r="H7" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
@@ -2037,7 +2037,7 @@
       </c>
       <c r="H8" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
@@ -2057,7 +2057,7 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
@@ -2075,7 +2075,7 @@
       </c>
       <c r="H10" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="3" t="s">
         <v>27</v>
       </c>
@@ -2095,7 +2095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="3" t="s">
         <v>27</v>
       </c>
@@ -2113,7 +2113,7 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="3" t="s">
         <v>27</v>
       </c>
@@ -2133,7 +2133,7 @@
       </c>
       <c r="H13" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="3" t="s">
         <v>27</v>
       </c>
@@ -2151,7 +2151,7 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="3" t="s">
         <v>27</v>
       </c>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="H15" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="3" t="s">
         <v>27</v>
       </c>
@@ -2187,7 +2187,7 @@
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="3" t="s">
         <v>27</v>
       </c>
@@ -2205,7 +2205,7 @@
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="3" t="s">
         <v>27</v>
       </c>
@@ -2225,7 +2225,7 @@
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="3" t="s">
         <v>27</v>
       </c>
@@ -2243,7 +2243,7 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="3" t="s">
         <v>27</v>
       </c>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="H20" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="3" t="s">
         <v>51</v>
       </c>
@@ -2281,7 +2281,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="3" t="s">
         <v>54</v>
       </c>
@@ -2301,7 +2301,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="3" t="s">
         <v>54</v>
       </c>
@@ -2321,7 +2321,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="3" t="s">
         <v>54</v>
       </c>
@@ -2341,7 +2341,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="3" t="s">
         <v>54</v>
       </c>
@@ -2361,7 +2361,7 @@
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="3" t="s">
         <v>54</v>
       </c>
@@ -2379,7 +2379,7 @@
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="3" t="s">
         <v>54</v>
       </c>

</xml_diff>